<commit_message>
update DOCS: add user page testing procedure
</commit_message>
<xml_diff>
--- a/DOCS.xlsx
+++ b/DOCS.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\Documents\github\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BB6DE35-03C8-4A71-83D8-973D733B5D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B389D595-C4A1-4CC2-8DCA-EFC2F548DF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" r:id="rId1"/>
     <sheet name="ATP" sheetId="2" r:id="rId2"/>
     <sheet name="specification" sheetId="3" r:id="rId3"/>
+    <sheet name="test User page" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tasks!$A$20:$G$31</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="202">
   <si>
     <t>Task</t>
   </si>
@@ -314,12 +315,6 @@
     <t>code</t>
   </si>
   <si>
-    <t>code version control must be used</t>
-  </si>
-  <si>
-    <t>build tool must be used</t>
-  </si>
-  <si>
     <t>code should apply most efficient algorithms</t>
   </si>
   <si>
@@ -441,6 +436,209 @@
   </si>
   <si>
     <t xml:space="preserve">user can see past (supplied) and present orders </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>code version control must be applied</t>
+  </si>
+  <si>
+    <t>build tool must be applied</t>
+  </si>
+  <si>
+    <t>instruction</t>
+  </si>
+  <si>
+    <t>1. log on to final_project and press 'sign in'</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>1. website shows on browser</t>
+  </si>
+  <si>
+    <t>2. user name and user password are shown</t>
+  </si>
+  <si>
+    <t>3. browser redirect to 'user-page', and user name is displayed in the upper right corner</t>
+  </si>
+  <si>
+    <t>1. log on to final_project and press 'register (sign up)'</t>
+  </si>
+  <si>
+    <t>2. fill user name nickname and user password</t>
+  </si>
+  <si>
+    <t>3. hit enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+3. hit enter</t>
+  </si>
+  <si>
+    <t>2. fill user name and user password</t>
+  </si>
+  <si>
+    <t>2. user name and email are shown</t>
+  </si>
+  <si>
+    <t>3. browser stays on 'home-page', and message have been sent to user</t>
+  </si>
+  <si>
+    <t>1. log on to final_project and press subscribe'</t>
+  </si>
+  <si>
+    <t>2. fill user name and email address</t>
+  </si>
+  <si>
+    <t>1. log on to final_project and press 'new  order'</t>
+  </si>
+  <si>
+    <t>2. fill ALL (*) marked fields</t>
+  </si>
+  <si>
+    <t>open web.xml and search for 'security protocol'</t>
+  </si>
+  <si>
+    <t>security protocol' has non empty string</t>
+  </si>
+  <si>
+    <t>1. sign in to website with user and password</t>
+  </si>
+  <si>
+    <t>1. user page shows 'you are connected as' at the top with user name</t>
+  </si>
+  <si>
+    <t>2. navigate to 'messages' and hit 'more'</t>
+  </si>
+  <si>
+    <t>2. menu opens with few options</t>
+  </si>
+  <si>
+    <t>3. choose 'new'</t>
+  </si>
+  <si>
+    <t>3. an upload file area and text area shows on page with 'send' 'cancel' buttons</t>
+  </si>
+  <si>
+    <t>4. choose an image of .png format and write 'this text' text, press 'send'</t>
+  </si>
+  <si>
+    <t>4. the message is shown on the user messages area, and the upload area disappears</t>
+  </si>
+  <si>
+    <t>5. choose an image of .png format and write 'this text' text, press 'send'</t>
+  </si>
+  <si>
+    <t>5. the message is shown on the user messages area, and the upload area disappears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. navigate to 'messages' </t>
+  </si>
+  <si>
+    <t>pre condition</t>
+  </si>
+  <si>
+    <t>user has at least 1 incoming message</t>
+  </si>
+  <si>
+    <t>3. choose 'reply'</t>
+  </si>
+  <si>
+    <t>2. at least 1 incoming message exist</t>
+  </si>
+  <si>
+    <t>registered user</t>
+  </si>
+  <si>
+    <t>1. navigate to 'messages'</t>
+  </si>
+  <si>
+    <t>1. a 'welcome' message from admin exist WITHOUT 'reply' option</t>
+  </si>
+  <si>
+    <t>2. at least 1 incoming message exist NOT from 'admin'</t>
+  </si>
+  <si>
+    <t>3. choose 'hide'</t>
+  </si>
+  <si>
+    <t>3. message disappears from 'messages' area</t>
+  </si>
+  <si>
+    <t>4. hit ctrl + F5 key</t>
+  </si>
+  <si>
+    <t>4. the chosen messages remains unseen</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. all messages remains </t>
+  </si>
+  <si>
+    <t>3. choose 'hide' from message body options</t>
+  </si>
+  <si>
+    <t>5. from the 'more' drop down menu choose 'show all messages'</t>
+  </si>
+  <si>
+    <t>6. hit ctrl + F5 key</t>
+  </si>
+  <si>
+    <t>5. hiden messages reappear</t>
+  </si>
+  <si>
+    <t>6. messages remain</t>
+  </si>
+  <si>
+    <t>at least 1 message sent by user exist</t>
+  </si>
+  <si>
+    <t>3. choose 'show sent messages' from drop down menu</t>
+  </si>
+  <si>
+    <t>2. at least 1 outgoing message exist from user</t>
+  </si>
+  <si>
+    <t>3. only messages sent from sign in user present</t>
+  </si>
+  <si>
+    <t>user can see all revieved messages according to sending user (incoming)</t>
+  </si>
+  <si>
+    <t>at least 2 message sent by 2 other users exists</t>
+  </si>
+  <si>
+    <t>2. at least 2 coming messages exist from 2 different users</t>
+  </si>
+  <si>
+    <t>3. click on the name of the sending user, in the message body</t>
+  </si>
+  <si>
+    <t>3. only messages sent from selected user appears</t>
+  </si>
+  <si>
+    <t>3. click on the OTHER name of the sending user, in the message body</t>
+  </si>
+  <si>
+    <t>5. only messages sent from selected user appears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user can place new order(s) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. navigate to 'orders' </t>
+  </si>
+  <si>
+    <t>2. at least 1 order exists with:
+order number, products and quantity, supplied</t>
+  </si>
+  <si>
+    <t>at least 1 order exists</t>
   </si>
 </sst>
 </file>
@@ -562,7 +760,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -607,11 +805,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -746,6 +1034,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -764,21 +1067,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -793,6 +1081,120 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1101,17 +1503,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48">
         <v>35</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="48"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
@@ -1141,7 +1543,7 @@
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="49" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1164,7 +1566,7 @@
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="11" t="s">
         <v>39</v>
       </c>
@@ -1185,7 +1587,7 @@
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="11" t="s">
         <v>40</v>
       </c>
@@ -1206,7 +1608,7 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -1217,7 +1619,7 @@
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="11" t="s">
         <v>42</v>
       </c>
@@ -1238,7 +1640,7 @@
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="11" t="s">
         <v>41</v>
       </c>
@@ -1259,18 +1661,18 @@
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="52"/>
       <c r="G9" s="13"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="58" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1295,7 +1697,7 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
@@ -1318,7 +1720,7 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
@@ -1341,7 +1743,7 @@
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
@@ -1364,7 +1766,7 @@
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="58"/>
       <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
@@ -1385,7 +1787,7 @@
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="A15" s="58"/>
       <c r="B15" s="11" t="s">
         <v>15</v>
       </c>
@@ -1406,7 +1808,7 @@
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="11" t="s">
         <v>7</v>
       </c>
@@ -1427,7 +1829,7 @@
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="11" t="s">
         <v>55</v>
       </c>
@@ -1448,7 +1850,7 @@
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
@@ -1469,18 +1871,18 @@
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="57"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58"/>
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="52"/>
       <c r="G19" s="13"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="50" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1505,7 +1907,7 @@
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="7" t="s">
         <v>18</v>
       </c>
@@ -1528,7 +1930,7 @@
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="7" t="s">
         <v>19</v>
       </c>
@@ -1551,7 +1953,7 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="11" t="s">
         <v>20</v>
       </c>
@@ -1572,7 +1974,7 @@
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="11" t="s">
         <v>21</v>
       </c>
@@ -1593,7 +1995,7 @@
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="7" t="s">
         <v>22</v>
       </c>
@@ -1616,7 +2018,7 @@
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
@@ -1639,7 +2041,7 @@
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="9" t="s">
         <v>51</v>
       </c>
@@ -1660,7 +2062,7 @@
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="7" t="s">
         <v>53</v>
       </c>
@@ -1683,7 +2085,7 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="7" t="s">
         <v>52</v>
       </c>
@@ -1706,7 +2108,7 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="7" t="s">
         <v>42</v>
       </c>
@@ -1729,7 +2131,7 @@
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="11" t="s">
         <v>23</v>
       </c>
@@ -1750,18 +2152,18 @@
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="49"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54"/>
       <c r="G32" s="13"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="56" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="11" t="s">
@@ -1784,7 +2186,7 @@
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="51"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="11" t="s">
         <v>25</v>
       </c>
@@ -1805,7 +2207,7 @@
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="51"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="11" t="s">
         <v>26</v>
       </c>
@@ -1826,7 +2228,7 @@
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="11" t="s">
         <v>27</v>
       </c>
@@ -1847,7 +2249,7 @@
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="51"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="11" t="s">
         <v>35</v>
       </c>
@@ -1868,7 +2270,7 @@
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="51"/>
+      <c r="A38" s="56"/>
       <c r="B38" s="11" t="s">
         <v>34</v>
       </c>
@@ -1889,7 +2291,7 @@
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
+      <c r="A39" s="56"/>
       <c r="B39" s="11" t="s">
         <v>28</v>
       </c>
@@ -1910,7 +2312,7 @@
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="11" t="s">
         <v>11</v>
       </c>
@@ -1931,18 +2333,18 @@
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
+      <c r="A41" s="55"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
       <c r="G41" s="13"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="52" t="s">
+      <c r="A42" s="57" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="11" t="s">
@@ -1965,7 +2367,7 @@
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="52"/>
+      <c r="A43" s="57"/>
       <c r="B43" s="11" t="s">
         <v>6</v>
       </c>
@@ -1986,7 +2388,7 @@
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="52"/>
+      <c r="A44" s="57"/>
       <c r="B44" s="11" t="s">
         <v>36</v>
       </c>
@@ -2007,7 +2409,7 @@
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="52"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="11" t="s">
         <v>37</v>
       </c>
@@ -2028,7 +2430,7 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="52"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="11"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
@@ -2135,17 +2537,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A10:A18"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A20:A31"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A10:A18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2167,15 +2569,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2199,10 +2601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F1C7CD-19A3-4E4C-8995-F8BF8AD34968}">
-  <dimension ref="A2:D80"/>
+  <dimension ref="A2:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,13 +2620,13 @@
         <v>66</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>67</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -2336,7 +2738,7 @@
         <v>76</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2346,7 +2748,7 @@
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2356,7 +2758,7 @@
       </c>
       <c r="C15" s="36"/>
       <c r="D15" s="33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2395,7 +2797,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D19" s="33"/>
     </row>
@@ -2406,7 +2808,7 @@
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2416,7 +2818,7 @@
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2426,7 +2828,7 @@
       </c>
       <c r="C22" s="35"/>
       <c r="D22" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2436,7 +2838,7 @@
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2445,7 +2847,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D24" s="33"/>
     </row>
@@ -2456,7 +2858,7 @@
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2466,7 +2868,7 @@
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2476,7 +2878,7 @@
       </c>
       <c r="C27" s="35"/>
       <c r="D27" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2485,7 +2887,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D28" s="33"/>
     </row>
@@ -2495,7 +2897,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D29" s="33"/>
     </row>
@@ -2505,7 +2907,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D30" s="33"/>
     </row>
@@ -2515,7 +2917,7 @@
         <v>9</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D31" s="33"/>
     </row>
@@ -2525,31 +2927,31 @@
         <v>10</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D32" s="33"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="34">
         <v>11</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D33" s="33"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="B34" s="34"/>
       <c r="C34" s="35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="34"/>
       <c r="C35" s="35"/>
@@ -2557,39 +2959,42 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="34"/>
       <c r="C36" s="35"/>
       <c r="D36" s="33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="34"/>
       <c r="C37" s="35"/>
       <c r="D37" s="33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="60"/>
       <c r="B38" s="34"/>
       <c r="C38" s="35"/>
       <c r="D38" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="G38" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="60"/>
       <c r="B39" s="34"/>
       <c r="C39" s="35"/>
       <c r="D39" s="33" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="60"/>
       <c r="B40" s="34"/>
       <c r="C40" s="35"/>
@@ -2597,27 +3002,27 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="60"/>
       <c r="B41" s="34"/>
       <c r="C41" s="35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D41" s="33"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="B42" s="34"/>
       <c r="C42" s="35"/>
       <c r="D42" s="33"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="62"/>
       <c r="B43" s="62"/>
       <c r="C43" s="62"/>
       <c r="D43" s="62"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="61" t="s">
         <v>33</v>
       </c>
@@ -2629,7 +3034,7 @@
       </c>
       <c r="D44" s="39"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="61"/>
       <c r="B45" s="37">
         <v>5</v>
@@ -2639,7 +3044,7 @@
       </c>
       <c r="D45" s="39"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="61"/>
       <c r="B46" s="37">
         <v>6</v>
@@ -2649,7 +3054,7 @@
       </c>
       <c r="D46" s="39"/>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
       <c r="B47" s="37">
         <v>7</v>
@@ -2659,7 +3064,7 @@
       </c>
       <c r="D47" s="39"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="61"/>
       <c r="B48" s="37">
         <v>8</v>
@@ -2735,7 +3140,7 @@
         <v>9</v>
       </c>
       <c r="C55" s="41" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="D55" s="42"/>
     </row>
@@ -2745,7 +3150,7 @@
         <v>10</v>
       </c>
       <c r="C56" s="41" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="D56" s="42"/>
     </row>
@@ -2755,7 +3160,7 @@
         <v>11</v>
       </c>
       <c r="C57" s="41" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D57" s="42"/>
     </row>
@@ -2765,7 +3170,7 @@
         <v>12</v>
       </c>
       <c r="C58" s="41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D58" s="42"/>
     </row>
@@ -2775,7 +3180,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D59" s="42"/>
     </row>
@@ -2785,7 +3190,7 @@
         <v>14</v>
       </c>
       <c r="C60" s="41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D60" s="42"/>
     </row>
@@ -2803,7 +3208,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D62" s="45"/>
     </row>
@@ -2814,7 +3219,7 @@
       </c>
       <c r="C63" s="44"/>
       <c r="D63" s="45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2824,7 +3229,7 @@
       </c>
       <c r="C64" s="44"/>
       <c r="D64" s="45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2834,7 +3239,7 @@
       </c>
       <c r="C65" s="44"/>
       <c r="D65" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2842,14 +3247,14 @@
       <c r="B66" s="43"/>
       <c r="C66" s="44"/>
       <c r="D66" s="45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="63"/>
       <c r="B67" s="43"/>
       <c r="C67" s="44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D67" s="45"/>
     </row>
@@ -2858,7 +3263,7 @@
       <c r="B68" s="43"/>
       <c r="C68" s="44"/>
       <c r="D68" s="45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2866,7 +3271,7 @@
       <c r="B69" s="43"/>
       <c r="C69" s="44"/>
       <c r="D69" s="47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2875,7 +3280,7 @@
         <v>2</v>
       </c>
       <c r="C70" s="44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D70" s="45"/>
     </row>
@@ -2884,7 +3289,7 @@
       <c r="B71" s="43"/>
       <c r="C71" s="44"/>
       <c r="D71" s="45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2892,7 +3297,7 @@
       <c r="B72" s="43"/>
       <c r="C72" s="44"/>
       <c r="D72" s="45" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,7 +3305,7 @@
       <c r="B73" s="43"/>
       <c r="C73" s="44"/>
       <c r="D73" s="45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2909,7 +3314,7 @@
         <v>3</v>
       </c>
       <c r="C74" s="44" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D74" s="45"/>
     </row>
@@ -2917,7 +3322,7 @@
       <c r="A75" s="63"/>
       <c r="B75" s="43"/>
       <c r="C75" s="44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D75" s="45"/>
     </row>
@@ -2927,7 +3332,7 @@
         <v>4</v>
       </c>
       <c r="C76" s="44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D76" s="45"/>
     </row>
@@ -2937,10 +3342,10 @@
         <v>5</v>
       </c>
       <c r="C77" s="46" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D77" s="45" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2948,7 +3353,7 @@
       <c r="B78" s="43"/>
       <c r="C78" s="44"/>
       <c r="D78" s="45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2956,7 +3361,7 @@
       <c r="B79" s="43"/>
       <c r="C79" s="44"/>
       <c r="D79" s="45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2976,4 +3381,575 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE0036B-A306-43EE-A865-F9C867BB9A87}">
+  <dimension ref="A2:D50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.140625" style="64" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="64" customWidth="1"/>
+    <col min="3" max="3" width="70.85546875" style="64" customWidth="1"/>
+    <col min="4" max="4" width="79.85546875" style="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="94"/>
+      <c r="C3" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="70"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="71"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="67" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="83" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="90"/>
+      <c r="C6" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="75" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="84"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="76" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="85"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="90"/>
+      <c r="C9" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="84"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="85"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="79" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="83" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="90"/>
+      <c r="C12" s="65" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="65" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="84"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="85"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="86" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="86"/>
+      <c r="C15" s="80" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="81" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="90"/>
+      <c r="C16" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="87" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="84"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="88" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="88" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="84"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="88" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="88" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="84"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="88" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="88" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="85"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="87" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="84"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="88" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="84"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="88" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="88" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="84"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="88" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" s="88" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="85"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="86" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="80" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="86" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="86"/>
+      <c r="C27" s="99" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="99" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="96"/>
+      <c r="C28" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="87" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="84"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" s="88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="84"/>
+      <c r="B30" s="97"/>
+      <c r="C30" s="88" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" s="88" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="85"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="89" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" s="89" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="83" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="96"/>
+      <c r="C32" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="87" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="84"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" s="88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="84"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="D34" s="88" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="84"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="88" t="s">
+        <v>178</v>
+      </c>
+      <c r="D35" s="88" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="84"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="88" t="s">
+        <v>183</v>
+      </c>
+      <c r="D36" s="88" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="85"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="89" t="s">
+        <v>184</v>
+      </c>
+      <c r="D37" s="82" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="83" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="96" t="s">
+        <v>187</v>
+      </c>
+      <c r="C38" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="87" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="84"/>
+      <c r="B39" s="97"/>
+      <c r="C39" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="88" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="84"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="88" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" s="88" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="84"/>
+      <c r="B41" s="98"/>
+      <c r="C41" s="89" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="89" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="83" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" s="93" t="s">
+        <v>192</v>
+      </c>
+      <c r="C42" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="87" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="84"/>
+      <c r="B43" s="101"/>
+      <c r="C43" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" s="88" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="84"/>
+      <c r="B44" s="101"/>
+      <c r="C44" s="88" t="s">
+        <v>194</v>
+      </c>
+      <c r="D44" s="88" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="84"/>
+      <c r="B45" s="101"/>
+      <c r="C45" s="88" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" s="88" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="85"/>
+      <c r="B46" s="100"/>
+      <c r="C46" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="D46" s="89" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="96" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" s="87" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="98"/>
+      <c r="B48" s="98"/>
+      <c r="C48" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="67" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="86" t="s">
+        <v>198</v>
+      </c>
+      <c r="B49" s="86"/>
+      <c r="C49" s="99" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="99" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="86" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="78"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>